<commit_message>
HOTFIX: changed calc logic. need fix
</commit_message>
<xml_diff>
--- a/input_files/storage/constr/6_constructor_rep_liab_analysis.xlsx
+++ b/input_files/storage/constr/6_constructor_rep_liab_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bitoche\REPOS\USER\dissertation_project\input_files\constructors\demo1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buyak\OneDrive\Рабочий стол\Андрюля\!DEVELOPER\dissertation_project\input_files\storage\constr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B58566-EA2E-495E-878C-E41A83C57504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25C4DEC-1835-4437-ACD8-E62689374C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constructor" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Аналитический разрез</t>
   </si>
@@ -186,6 +184,9 @@
   </si>
   <si>
     <t>ACTIVE, OBLIGATE</t>
+  </si>
+  <si>
+    <t>loss_component == 'компонент убытка'</t>
   </si>
 </sst>
 </file>
@@ -272,9 +273,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -283,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -627,18 +628,18 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.375" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -652,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -666,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -680,266 +681,266 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="B17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="8" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="8" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -953,7 +954,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A3:D3 D4:D12" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C1 A3:D3 D4:D11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>